<commit_message>
I created a detailed analysis for different types of weather, and I conducted an analysis by state.
</commit_message>
<xml_diff>
--- a/statistic_weather.xlsx
+++ b/statistic_weather.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1ad46d03d4d252f/Pulpit/Data Hunters/jdszr9-data_hunters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{9059AEE9-18F1-435A-A886-150F0B486B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8B3A069-05FA-467F-B5AF-F6BD4F566414}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{9059AEE9-18F1-435A-A886-150F0B486B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43C8BED0-4B84-47EE-A930-C9CFF84AEEE6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A236FD18-E3B1-4B18-AC3D-B9FE5C5E7EB6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A236FD18-E3B1-4B18-AC3D-B9FE5C5E7EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -41,30 +41,6 @@
     <t>Type of Day</t>
   </si>
   <si>
-    <t>Fog</t>
-  </si>
-  <si>
-    <t>Thunder</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>Outlier</t>
-  </si>
-  <si>
-    <t>Dust</t>
-  </si>
-  <si>
-    <t>Tornado</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Ordinary</t>
-  </si>
-  <si>
     <t>Number accidents</t>
   </si>
   <si>
@@ -77,10 +53,34 @@
     <t>Number days</t>
   </si>
   <si>
-    <t>Number accounts per day</t>
-  </si>
-  <si>
     <t>Number accidents per days_air</t>
+  </si>
+  <si>
+    <t>all_days</t>
+  </si>
+  <si>
+    <t>ordinary_days</t>
+  </si>
+  <si>
+    <t>outlier_days</t>
+  </si>
+  <si>
+    <t>fog_days</t>
+  </si>
+  <si>
+    <t>thunder_days</t>
+  </si>
+  <si>
+    <t>calm_days</t>
+  </si>
+  <si>
+    <t>snow_days</t>
+  </si>
+  <si>
+    <t>big_snow_days</t>
+  </si>
+  <si>
+    <t>dust_days</t>
   </si>
 </sst>
 </file>
@@ -117,9 +117,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -438,51 +437,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA94B69-3ECB-49AB-81FA-C259806EF421}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2.1375715116144201</v>
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2.1375000000000002</v>
       </c>
       <c r="C2">
         <v>2845342</v>
@@ -493,172 +490,168 @@
       <c r="E2">
         <v>2099</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>4.8600000000000003</v>
       </c>
-      <c r="G2">
-        <v>1.355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2.1336851569638902</v>
+      </c>
+      <c r="C3">
+        <v>2727124</v>
+      </c>
+      <c r="D3">
+        <v>545106</v>
+      </c>
+      <c r="E3">
+        <v>2097</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.13542335220487</v>
-      </c>
-      <c r="C3">
-        <v>2751586</v>
-      </c>
-      <c r="D3">
-        <v>555094</v>
-      </c>
-      <c r="E3">
-        <v>2099</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4.96</v>
-      </c>
-      <c r="G3">
-        <v>1.31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>2.0857735300426601</v>
+      </c>
+      <c r="C4">
+        <v>629355</v>
+      </c>
+      <c r="D4">
+        <v>67897</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4">
+        <v>9.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
         <v>2.0584002002530899</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>287636</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>28310</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>1862</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5">
         <v>10.16</v>
       </c>
-      <c r="G4">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.0799746450304202</v>
-      </c>
-      <c r="C5">
-        <v>197200</v>
-      </c>
-      <c r="D5">
-        <v>16613</v>
-      </c>
-      <c r="E5">
-        <v>1599</v>
-      </c>
-      <c r="F5" s="1">
-        <v>11.87</v>
-      </c>
-      <c r="G5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2.1160346579665101</v>
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2.0859349602209099</v>
       </c>
       <c r="C6">
-        <v>37394</v>
+        <v>279921</v>
       </c>
       <c r="D6">
-        <v>3628</v>
+        <v>26462</v>
       </c>
       <c r="E6">
-        <v>630</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10.31</v>
-      </c>
-      <c r="G6">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1814</v>
+      </c>
+      <c r="F6">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2.0929741151611099</v>
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2.43364142278093</v>
       </c>
       <c r="C7">
-        <v>1893</v>
+        <v>226233</v>
       </c>
       <c r="D7">
-        <v>182</v>
+        <v>88907</v>
       </c>
       <c r="E7">
-        <v>129</v>
-      </c>
-      <c r="F7" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="G7">
+        <v>1125</v>
+      </c>
+      <c r="F7">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2.1510255595055701</v>
+      </c>
+      <c r="C8">
+        <v>103797</v>
+      </c>
+      <c r="D8">
+        <v>15376</v>
+      </c>
+      <c r="E8">
+        <v>950</v>
+      </c>
+      <c r="F8">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2.1350464734827699</v>
+      </c>
+      <c r="C9">
+        <v>25606</v>
+      </c>
+      <c r="D9">
+        <v>2493</v>
+      </c>
+      <c r="E9">
+        <v>541</v>
+      </c>
+      <c r="F9">
+        <v>10.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2.0929741151611099</v>
-      </c>
-      <c r="C8">
-        <v>1893</v>
-      </c>
-      <c r="D8">
-        <v>182</v>
-      </c>
-      <c r="E8">
-        <v>129</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="G8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
+      <c r="B10">
+        <v>2.0911917098445501</v>
+      </c>
+      <c r="C10">
+        <v>1930</v>
+      </c>
+      <c r="D10">
+        <v>185</v>
+      </c>
+      <c r="E10">
+        <v>132</v>
+      </c>
+      <c r="F10">
+        <v>10.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>